<commit_message>
updating methods for different semantic spaces
</commit_message>
<xml_diff>
--- a/novelty_scoring/autdata_official_ratings_johnhenry.xlsx
+++ b/novelty_scoring/autdata_official_ratings_johnhenry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhec8\Documents\Northwestern_SROP\AUT-Scoring\novelty_scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF50DA7-8339-4957-8BE5-E859C13ED742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D43F86-2E36-4B34-9EE6-FC077D397A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2310" yWindow="2490" windowWidth="21570" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8094,8 +8094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D395"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D175" sqref="D175"/>
+    <sheetView tabSelected="1" topLeftCell="A373" workbookViewId="0">
+      <selection activeCell="D193" sqref="D193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13624,8 +13624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D403"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A391" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19272,8 +19272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D461"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D462" sqref="D462"/>
+    <sheetView topLeftCell="A442" workbookViewId="0">
+      <selection activeCell="D339" sqref="D339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20257,6 +20257,9 @@
       <c r="C70" t="s">
         <v>760</v>
       </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -25723,8 +25726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D491"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K485" sqref="K485"/>
+    <sheetView topLeftCell="A478" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D315" sqref="D315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32597,8 +32600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D425"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A418" workbookViewId="0">
+      <selection activeCell="D381" sqref="D381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38547,8 +38550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D439"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D129" sqref="D129"/>
+    <sheetView topLeftCell="A418" workbookViewId="0">
+      <selection activeCell="D430" sqref="D430"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44696,8 +44699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D454"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView topLeftCell="A436" workbookViewId="0">
+      <selection activeCell="D301" sqref="D301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51055,8 +51058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D448"/>
   <sheetViews>
-    <sheetView topLeftCell="A425" workbookViewId="0">
-      <selection activeCell="D449" sqref="D449"/>
+    <sheetView topLeftCell="A427" workbookViewId="0">
+      <selection activeCell="D348" sqref="D348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>